<commit_message>
Una prueba con la interfaz grafica
</commit_message>
<xml_diff>
--- a/Datos/AREAS_INFANTILES_2019.xlsx
+++ b/Datos/AREAS_INFANTILES_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\GitHub\ideas\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E6FE73-B8D9-4D7C-9CB6-D094D0103D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5212B26A-A84B-433F-AB63-67E0F83EB8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" tabRatio="142" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23252" uniqueCount="7428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23253" uniqueCount="7429">
   <si>
     <t>MXASSETNUM,C,12</t>
   </si>
@@ -22304,6 +22304,9 @@
   </si>
   <si>
     <t>nueva linea incluida</t>
+  </si>
+  <si>
+    <t>Cambio una celda</t>
   </si>
 </sst>
 </file>
@@ -22658,10 +22661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1966"/>
+  <dimension ref="A1:N1967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1939" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1967" sqref="A1967"/>
+    <sheetView tabSelected="1" topLeftCell="A1940" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1968" sqref="B1968"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -108056,6 +108059,11 @@
         <v>7427</v>
       </c>
     </row>
+    <row r="1967" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1967" t="s">
+        <v>7428</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>